<commit_message>
read file and mapto json
</commit_message>
<xml_diff>
--- a/seed_files/แบบสำหรับนำข้อมูลเข้า.xlsx
+++ b/seed_files/แบบสำหรับนำข้อมูลเข้า.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken/Desktop/api-file-excel-sandbox/seed_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C64E1B64-4235-41CE-94FF-FD50E86D0EF9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65881ED3-8295-014F-9828-2F0377430D61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="21570" windowHeight="7980"/>
+    <workbookView xWindow="2740" yWindow="5100" windowWidth="26060" windowHeight="10340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="รายละเอียด" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>ชื่อจริง</t>
   </si>
@@ -117,9 +117,6 @@
     <t>เหล่าวินัย</t>
   </si>
   <si>
-    <t>27/03/02</t>
-  </si>
-  <si>
     <t>ปวช</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>3. บันทึก การแก้ไข ไฟล์นี้แล้วอัพโหลดไปทีหน้าเว็บไซท์</t>
   </si>
   <si>
-    <t>22/02/08</t>
-  </si>
-  <si>
     <t>ประถม</t>
   </si>
   <si>
@@ -145,6 +139,31 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">ใส่ตัวอักษรนามสกุลของนักเรียน เช่น </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ชาติดำรงค์</t>
+    </r>
+  </si>
+  <si>
+    <t>รูปแบบของการศึกษา</t>
+  </si>
+  <si>
+    <t>ปวส</t>
+  </si>
+  <si>
+    <t>สำหรับคัดลอกรูปแบบการศึกษา เพื่อนำไปใช้งาน</t>
+  </si>
+  <si>
+    <r>
       <t>ใส่วันเกิดเป็นรูปแบบ</t>
     </r>
     <r>
@@ -155,7 +174,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> วัน/เดือน/ปีคศ. 2 หลักสุดท้าย</t>
+      <t xml:space="preserve"> วัน/เดือน/ปีคศ. 4 หลัก</t>
     </r>
     <r>
       <rPr>
@@ -175,7 +194,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>01/01/96</t>
+      <t>01/01/1996</t>
     </r>
     <r>
       <rPr>
@@ -196,32 +215,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ใส่ตัวอักษรนามสกุลของนักเรียน เช่น </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>2000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>เลือก</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ชาติดำรงค์</t>
-    </r>
-  </si>
-  <si>
-    <t>รูปแบบของการศึกษา</t>
-  </si>
-  <si>
-    <t>ปวส</t>
-  </si>
-  <si>
+      <t>ระดับการศึกษา</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -230,7 +247,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>เลือก</t>
+      <t xml:space="preserve"> 1 ใน 4 </t>
     </r>
     <r>
       <rPr>
@@ -240,7 +257,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ระดับการศึกษา</t>
+      <t xml:space="preserve">คำนี้ </t>
     </r>
     <r>
       <rPr>
@@ -250,7 +267,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 1 ใน 4 </t>
+      <t>และไม่ใส่จุด</t>
     </r>
     <r>
       <rPr>
@@ -260,7 +277,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">คำนี้ </t>
+      <t xml:space="preserve"> เท่านั้น </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ปวส</t>
     </r>
     <r>
       <rPr>
@@ -270,17 +297,17 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>และไม่ใส่จุด</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> เท่านั้น </t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ปวช</t>
     </r>
     <r>
       <rPr>
@@ -290,18 +317,45 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>ปวส ปวช มัธยม ประถม</t>
-    </r>
-  </si>
-  <si>
-    <t>สำหรับคัดลอกรูปแบบการศึกษา เพื่อนำไปใช้งาน</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>มัธยม</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ประถม</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +377,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -428,6 +489,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,36 +526,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -780,153 +841,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="14"/>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="D3" s="9">
+      <c r="B3" s="14"/>
+      <c r="D3" s="4">
         <v>45663</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="5">
         <v>37231</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="4">
         <v>6</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="D4" s="4">
+        <v>306</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5">
+        <v>39500</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="D4" s="9">
-        <v>306</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="I4" s="4">
         <v>4</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="D5" s="9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="D5" s="4">
         <v>11235</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="5">
+        <v>37342</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="I5" s="4">
         <v>2</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="J5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -934,7 +995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,31 +1003,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -974,49 +1035,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="14"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="14"/>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1035,45 +1096,114 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>45663</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5">
+        <v>37231</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>306</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5">
+        <v>39500</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>11235</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5">
+        <v>37342</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>